<commit_message>
Memindahkan file dan merapikan struktur folder
</commit_message>
<xml_diff>
--- a/data_pengeluaran.xlsx
+++ b/data_pengeluaran.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,7 +589,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="n">
+      <c r="A9" s="2" t="n">
         <v>45796</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -603,6 +603,24 @@
       <c r="D9" t="inlineStr">
         <is>
           <t>pembelian air</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>45795</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Pengeluaran</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>800000</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Pupuk 50 liter</t>
         </is>
       </c>
     </row>

</xml_diff>